<commit_message>
export pdf and excel done, created a new component
</commit_message>
<xml_diff>
--- a/backend/web/storage/IMPORT-EKSPEDISI.xlsx
+++ b/backend/web/storage/IMPORT-EKSPEDISI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\revaldi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B821F3E9-B17E-4C52-BF29-EA7BDAFB6882}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43E7B72-C3D1-4D87-B827-A5FC0FD212C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="7995" xr2:uid="{9B83173F-6C7A-4860-9571-8D1D55DFF471}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="15375" windowHeight="7995" xr2:uid="{9B83173F-6C7A-4860-9571-8D1D55DFF471}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>(INTEGER)</t>
   </si>
   <si>
-    <t>Semarang</t>
+    <t>Balikpapan</t>
   </si>
 </sst>
 </file>
@@ -102,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,6 +111,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -433,7 +436,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,13 +465,13 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -497,14 +500,14 @@
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>36000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="1">
@@ -514,14 +517,14 @@
         <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>40000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1">
@@ -538,7 +541,7 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1">

</xml_diff>